<commit_message>
add bulk uplaod branchs
</commit_message>
<xml_diff>
--- a/public/sample files/sample data for branches data upload.xlsx
+++ b/public/sample files/sample data for branches data upload.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Praveen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\attendance-system\public\sample files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530323BE-41DF-44E6-8762-4C097988AF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE204823-4AD3-4EEE-B1B7-8017CFCB5A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>Branch Name</t>
   </si>
@@ -112,16 +112,29 @@
   </si>
   <si>
     <t>Barpali</t>
+  </si>
+  <si>
+    <t>important points*</t>
+  </si>
+  <si>
+    <t>1)first  letter should be capital of every word</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,8 +160,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,6 +679,16 @@
         <v>28.123560000000001</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>